<commit_message>
Clean up the repository
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garrett/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garrett/Dropbox/Files/1 - CS/Project/D-MAP/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E45698-0140-214D-8863-70EBC724AD29}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD546C08-062F-D541-AEFD-EDB47A7E7757}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{FBBFB87E-B1A1-8D46-96F8-8D7C5474BA15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{FBBFB87E-B1A1-8D46-96F8-8D7C5474BA15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="4">
   <si>
     <t>input-6.in</t>
   </si>
   <si>
     <t>input-7.in</t>
+  </si>
+  <si>
+    <t>D-MAP</t>
+  </si>
+  <si>
+    <t>Physical Limit</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
               <a:t>7-character Password Cracker</a:t>
             </a:r>
           </a:p>
@@ -199,23 +205,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$J$1:$J$5</c:f>
+              <c:f>Sheet1!$D$40:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -223,24 +244,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$7:$I$11</c:f>
+              <c:f>Sheet1!$C$40:$C$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>79.197857046127297</c:v>
+                  <c:v>460.91749153137198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.739047813415496</c:v>
+                  <c:v>230.432495689392</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.173595809936501</c:v>
+                  <c:v>160.993093013763</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.275656223297098</c:v>
+                  <c:v>115.71876797676001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.315134620666498</c:v>
+                  <c:v>93.710672187805102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.319495534896802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.859497928619305</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58.727485036849899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.323986530303898</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.586897420883098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,26 +318,80 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$1:$L$5</c:f>
+              <c:f>Sheet1!$E$40:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>458.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.428571428571431</c:v>
+                  <c:v>229.48500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>152.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>114.74250000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>91.794000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.495000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65.567142857142855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.371250000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.99666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.897000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,7 +443,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Number of Machines</a:t>
                 </a:r>
               </a:p>
@@ -437,6 +527,7 @@
         <c:axId val="109506623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="480"/>
           <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -475,19 +566,19 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> t</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>ime</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> to crack 10 passwords on five runs</a:t>
                 </a:r>
               </a:p>
@@ -496,10 +587,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> (Second)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -547,7 +638,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -585,6 +678,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.89247436482278508"/>
+          <c:y val="0.41985879374681506"/>
+          <c:w val="9.9968960114242653E-2"/>
+          <c:h val="0.14770404221392994"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -685,12 +788,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-Hans" b="1"/>
-              <a:t>6</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>-character Password Cracker</a:t>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>6-character Password Cracker</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -762,23 +861,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$J$1:$J$5</c:f>
+              <c:f>Sheet1!$D$40:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -786,24 +900,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$1:$I$5</c:f>
+              <c:f>Sheet1!$C$50:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.4626272201538004</c:v>
+                  <c:v>17.7815650939941</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4940308570861802</c:v>
+                  <c:v>8.8821872711181609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2970007419586098</c:v>
+                  <c:v>6.6817003250121996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3237367153167701</c:v>
+                  <c:v>4.50655498504638</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.28575773239135</c:v>
+                  <c:v>4.4595166683196998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4539082050323398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4984941959381102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2701476573943999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3410444736480698</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2843965530395498</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,7 +940,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C87-9241-A101-A2324E09C783}"/>
+              <c16:uniqueId val="{00000000-8895-614A-AB45-3EDF0DF157DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -845,26 +974,80 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$7:$L$11</c:f>
+              <c:f>Sheet1!$E$50:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.3333333333333335</c:v>
+                  <c:v>17.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>5.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.75</c:v>
+                  <c:v>4.335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.75</c:v>
+                  <c:v>3.468</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4771428571428573</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1675</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1675</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,7 +1055,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3C87-9241-A101-A2324E09C783}"/>
+              <c16:uniqueId val="{00000001-8895-614A-AB45-3EDF0DF157DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -916,7 +1099,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Number of Machines</a:t>
                 </a:r>
               </a:p>
@@ -1000,7 +1183,6 @@
         <c:axId val="109506623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1038,19 +1220,19 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> t</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>ime</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> to crack 10 passwords on five runs</a:t>
                 </a:r>
               </a:p>
@@ -1059,10 +1241,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> (Second)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1110,7 +1292,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1148,6 +1332,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.89738539142943674"/>
+          <c:y val="0.42612184176351653"/>
+          <c:w val="9.5403070109024837E-2"/>
+          <c:h val="0.14144099419722847"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2330,16 +2524,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2366,23 +2560,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C08AF1B-BA28-4D42-B52F-31393BDDEBFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{835FA2C1-0B34-0341-94AF-57405ADFF363}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2702,15 +2896,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF295B1F-F4FB-E443-AEAD-506F69FF7D0C}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2739,8 +2936,12 @@
         <f>360/6</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2769,8 +2970,12 @@
         <f>360/7</f>
         <v>51.428571428571431</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2799,8 +3004,12 @@
         <f>360/8</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2829,8 +3038,12 @@
         <f>360/9</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2859,8 +3072,12 @@
         <f>360/10</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2873,8 +3090,12 @@
       <c r="D6" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2903,8 +3124,12 @@
         <f>14/6</f>
         <v>2.3333333333333335</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2933,8 +3158,12 @@
         <f>14/7</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2963,8 +3192,12 @@
         <f>14/8</f>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -2993,8 +3226,12 @@
         <f>14/8</f>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
@@ -3011,8 +3248,436 @@
         <f>14/8</f>
         <v>1.75</v>
       </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>460.91749153137198</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <f>458.97/D40</f>
+        <v>458.97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1">
+        <v>230.432495689392</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" ref="E41:E48" si="0">458.97/D41</f>
+        <v>229.48500000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1">
+        <v>160.993093013763</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="0"/>
+        <v>152.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1">
+        <v>115.71876797676001</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>114.74250000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1">
+        <v>93.710672187805102</v>
+      </c>
+      <c r="D44" s="1">
+        <v>5</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="0"/>
+        <v>91.794000000000011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1">
+        <v>79.319495534896802</v>
+      </c>
+      <c r="D45" s="1">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="0"/>
+        <v>76.495000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1">
+        <v>71.859497928619305</v>
+      </c>
+      <c r="D46" s="1">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="0"/>
+        <v>65.567142857142855</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1">
+        <v>58.727485036849899</v>
+      </c>
+      <c r="D47" s="1">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="0"/>
+        <v>57.371250000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>57.323986530303898</v>
+      </c>
+      <c r="D48" s="1">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="0"/>
+        <v>50.99666666666667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1">
+        <v>50.586897420883098</v>
+      </c>
+      <c r="D49" s="1">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1">
+        <f>458.97/D49</f>
+        <v>45.897000000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1">
+        <v>17.7815650939941</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <f>17.34/D50</f>
+        <v>17.34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8.8821872711181609</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" ref="E51:E59" si="1">17.34/D51</f>
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1">
+        <v>6.6817003250121996</v>
+      </c>
+      <c r="D52" s="1">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <v>4.50655498504638</v>
+      </c>
+      <c r="D53" s="1">
+        <v>4</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>4.335</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1">
+        <v>4.4595166683196998</v>
+      </c>
+      <c r="D54" s="1">
+        <v>5</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="1"/>
+        <v>3.468</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>4.4539082050323398</v>
+      </c>
+      <c r="D55" s="1">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4.4984941959381102</v>
+      </c>
+      <c r="D56" s="1">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4771428571428573</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1">
+        <v>5</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2.2701476573943999</v>
+      </c>
+      <c r="D57" s="1">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1675</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2.3410444736480698</v>
+      </c>
+      <c r="D58" s="1">
+        <v>9</v>
+      </c>
+      <c r="E58" s="1">
+        <f>17.34/8</f>
+        <v>2.1675</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2.2843965530395498</v>
+      </c>
+      <c r="D59" s="1">
+        <v>10</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2.1675</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="N1:Q61">
+    <sortCondition descending="1" ref="N1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>